<commit_message>
changes to AFD tanks map
</commit_message>
<xml_diff>
--- a/UploadedFiles/AFDTanks.xlsx
+++ b/UploadedFiles/AFDTanks.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="AllTanks" sheetId="3" r:id="rId2"/>
+    <sheet name="Cities" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5386" uniqueCount="1827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="1884">
   <si>
     <t>coopid</t>
   </si>
@@ -5520,6 +5521,177 @@
   </si>
   <si>
     <t>EARL DEAN</t>
+  </si>
+  <si>
+    <t>ARLINGTON</t>
+  </si>
+  <si>
+    <t>AUGUSTA</t>
+  </si>
+  <si>
+    <t>BENNINGTON</t>
+  </si>
+  <si>
+    <t>BROOKVILLE</t>
+  </si>
+  <si>
+    <t>BURRTON</t>
+  </si>
+  <si>
+    <t>BUSHTON</t>
+  </si>
+  <si>
+    <t>CANTON</t>
+  </si>
+  <si>
+    <t>CHASE</t>
+  </si>
+  <si>
+    <t>CHENEY</t>
+  </si>
+  <si>
+    <t>CLAY CENTER</t>
+  </si>
+  <si>
+    <t>COTTONWOOD FALLS</t>
+  </si>
+  <si>
+    <t>DEARBORN</t>
+  </si>
+  <si>
+    <t>DOUGLAS</t>
+  </si>
+  <si>
+    <t>ENTERPRISE</t>
+  </si>
+  <si>
+    <t>GALVA</t>
+  </si>
+  <si>
+    <t>GENESEO</t>
+  </si>
+  <si>
+    <t>GOESSEL</t>
+  </si>
+  <si>
+    <t>GREAT BEND</t>
+  </si>
+  <si>
+    <t>GYPSUM</t>
+  </si>
+  <si>
+    <t>HAMILTON</t>
+  </si>
+  <si>
+    <t>HANNIBAL</t>
+  </si>
+  <si>
+    <t>HAVEN</t>
+  </si>
+  <si>
+    <t>HILLSBORO</t>
+  </si>
+  <si>
+    <t>JERSEY CITY</t>
+  </si>
+  <si>
+    <t>KANSAS CITY</t>
+  </si>
+  <si>
+    <t>KINGMAN</t>
+  </si>
+  <si>
+    <t>LANGDON</t>
+  </si>
+  <si>
+    <t>LENARDVILLE</t>
+  </si>
+  <si>
+    <t>LINDSBORG</t>
+  </si>
+  <si>
+    <t>LORRAINE</t>
+  </si>
+  <si>
+    <t>LYONS</t>
+  </si>
+  <si>
+    <t>MARION</t>
+  </si>
+  <si>
+    <t>MARQUETTE</t>
+  </si>
+  <si>
+    <t>MINNEAPOLIS</t>
+  </si>
+  <si>
+    <t>MULVANE</t>
+  </si>
+  <si>
+    <t>NEW CAMBRIA</t>
+  </si>
+  <si>
+    <t>NICKERSON</t>
+  </si>
+  <si>
+    <t>PARTRIDGE</t>
+  </si>
+  <si>
+    <t>PAWNEE ROCK</t>
+  </si>
+  <si>
+    <t>PRETTY PRAIRIE</t>
+  </si>
+  <si>
+    <t>ROMAONA</t>
+  </si>
+  <si>
+    <t>ROSE HILL</t>
+  </si>
+  <si>
+    <t>ROXBURY</t>
+  </si>
+  <si>
+    <t>SALINA</t>
+  </si>
+  <si>
+    <t>SEDGWICK</t>
+  </si>
+  <si>
+    <t>SMOLAN</t>
+  </si>
+  <si>
+    <t>STERLING</t>
+  </si>
+  <si>
+    <t>SYLVIA</t>
+  </si>
+  <si>
+    <t>TAMPA</t>
+  </si>
+  <si>
+    <t>TORONTO</t>
+  </si>
+  <si>
+    <t>TOWANDA</t>
+  </si>
+  <si>
+    <t>WAKEFIELD</t>
+  </si>
+  <si>
+    <t>WILSEY</t>
+  </si>
+  <si>
+    <t>WINDOM</t>
+  </si>
+  <si>
+    <t>WOODBINE</t>
+  </si>
+  <si>
+    <t>YODER</t>
+  </si>
+  <si>
+    <t>CITY</t>
   </si>
 </sst>
 </file>
@@ -5590,16 +5762,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -5737,15 +5940,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K1020" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K1020" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:K1020"/>
   <tableColumns count="11">
     <tableColumn id="1" name="coopid"/>
     <tableColumn id="2" name="customerid"/>
-    <tableColumn id="3" name="companyname" dataDxfId="3"/>
-    <tableColumn id="4" name="firstname" dataDxfId="2"/>
-    <tableColumn id="5" name="lastname" dataDxfId="1"/>
-    <tableColumn id="6" name="city" dataDxfId="0"/>
+    <tableColumn id="3" name="companyname" dataDxfId="6"/>
+    <tableColumn id="4" name="firstname" dataDxfId="5"/>
+    <tableColumn id="5" name="lastname" dataDxfId="4"/>
+    <tableColumn id="6" name="city" dataDxfId="3"/>
     <tableColumn id="7" name="siteid"/>
     <tableColumn id="8" name="long"/>
     <tableColumn id="9" name="lat"/>
@@ -5753,6 +5956,16 @@
     <tableColumn id="11" name="probeid"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:A106" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A106"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="CITY" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -6021,7 +6234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -6029,7 +6242,7 @@
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -9657,8 +9870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F46" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45347,4 +45560,557 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A1019">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>